<commit_message>
recruitment: user import fixed
</commit_message>
<xml_diff>
--- a/externals/recruitment/session_user_bundle.xlsx
+++ b/externals/recruitment/session_user_bundle.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,10 +13,260 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>NAMA</t>
+  </si>
+  <si>
+    <t>SEAT/TABLE</t>
+  </si>
+  <si>
+    <t>Putra Aa 1</t>
+  </si>
+  <si>
+    <t>Putra Aa 4</t>
+  </si>
+  <si>
+    <t>Putra Aa 5</t>
+  </si>
+  <si>
+    <t>Putra Aa 6</t>
+  </si>
+  <si>
+    <t>Putra Aa 7</t>
+  </si>
+  <si>
+    <t>Putra Aa 8</t>
+  </si>
+  <si>
+    <t>Putra Ab 2</t>
+  </si>
+  <si>
+    <t>Putra Ac 3</t>
+  </si>
+  <si>
+    <t>Putra Aa 2</t>
+  </si>
+  <si>
+    <t>Putra Ab 3</t>
+  </si>
+  <si>
+    <t>Putra Ac 4</t>
+  </si>
+  <si>
+    <t>Putra Aa 3</t>
+  </si>
+  <si>
+    <t>Putra Ab 4</t>
+  </si>
+  <si>
+    <t>Putra Ac 5</t>
+  </si>
+  <si>
+    <t>Putra Ab 5</t>
+  </si>
+  <si>
+    <t>Putra Ac 6</t>
+  </si>
+  <si>
+    <t>Putra Ab 6</t>
+  </si>
+  <si>
+    <t>Putra Ac 7</t>
+  </si>
+  <si>
+    <t>Putra Ab 7</t>
+  </si>
+  <si>
+    <t>Putra Ac 8</t>
+  </si>
+  <si>
+    <t>Putra Ab 8</t>
+  </si>
+  <si>
+    <t>Putra Ac 9</t>
+  </si>
+  <si>
+    <t>Putra Ab 9</t>
+  </si>
+  <si>
+    <t>Putra Ac 10</t>
+  </si>
+  <si>
+    <t>PLNCDUGM</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19001</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19002</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19003</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19004</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19005</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19006</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19007</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19008</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19009</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19010</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19011</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19012</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19013</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19014</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19015</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19016</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19017</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19018</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19019</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19020</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19021</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19022</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19023</t>
+  </si>
+  <si>
+    <t>PLNCDUGM19024</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>A24</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,14 +294,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +359,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +394,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +602,449 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="6" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>